<commit_message>
added cell value caching; vastly improved column name lookup speeds as result.
</commit_message>
<xml_diff>
--- a/test_resources/st_src_1_v_short.xlsx
+++ b/test_resources/st_src_1_v_short.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="50">
   <si>
     <t>col1</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
   </si>
 </sst>
 </file>
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN910"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,46 +1721,126 @@
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
-      <c r="AM11" s="1"/>
-      <c r="AN11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AM11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN11" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>

</xml_diff>